<commit_message>
PWA: manifest e service worker, fix numeri interi, aggiorno Excel e PNG loghi
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930E9F83-3B62-6E44-8078-D4F803E425CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D053ABA-7F13-EA43-8293-F5EA83DD59B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15160" windowHeight="15980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="54">
   <si>
     <t>Data</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Commerciali Ferramenta</t>
   </si>
   <si>
-    <t>Officina Ronconi</t>
-  </si>
-  <si>
     <t>Bar Caligo Spazio Kura</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>lacorte.png</t>
   </si>
   <si>
-    <t>ronconi.png</t>
-  </si>
-  <si>
     <t>commferr.png</t>
   </si>
   <si>
@@ -184,7 +178,13 @@
     <t>Monday, 7 July 2025</t>
   </si>
   <si>
-    <t>√</t>
+    <t>s</t>
+  </si>
+  <si>
+    <t>PM Sport</t>
+  </si>
+  <si>
+    <t>piemme.png</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="13">
         <v>0.85416666666666663</v>
@@ -663,13 +663,13 @@
         <v>31</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -735,7 +735,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -838,10 +838,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="I1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -851,7 +851,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -886,12 +886,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -918,13 +918,10 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -956,18 +953,15 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -994,10 +988,10 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1029,12 +1023,12 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -1064,12 +1058,12 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -1099,15 +1093,15 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
@@ -1134,12 +1128,12 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
@@ -1169,12 +1163,12 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -1204,7 +1198,12 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1216,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1270,13 +1269,13 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -1293,16 +1292,16 @@
         <v>27</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -1322,13 +1321,13 @@
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -1348,13 +1347,13 @@
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
         <v>30</v>
@@ -1374,13 +1373,13 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
         <v>30</v>
@@ -1397,16 +1396,16 @@
         <v>28</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -1423,16 +1422,16 @@
         <v>27</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
         <v>30</v>
@@ -1452,13 +1451,13 @@
         <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H9" t="s">
         <v>30</v>
@@ -1475,16 +1474,16 @@
         <v>28</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
@@ -1492,7 +1491,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2">
         <v>0.85416666666666663</v>
@@ -1504,13 +1503,13 @@
         <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
         <v>30</v>
@@ -1518,7 +1517,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2">
         <v>0.89583333333333337</v>
@@ -1530,13 +1529,13 @@
         <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -1553,16 +1552,16 @@
         <v>28</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>32</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
         <v>30</v>
@@ -1582,13 +1581,13 @@
         <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -1608,13 +1607,13 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
         <v>30</v>
@@ -1634,13 +1633,13 @@
         <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H16" t="s">
         <v>30</v>
@@ -1660,13 +1659,13 @@
         <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H17" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Partite: solo calendario, tutte le card uguali, fix loghi, aggiorno Excel e PNG
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D053ABA-7F13-EA43-8293-F5EA83DD59B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B90272C-C8E9-F240-BAA4-938FB824FF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
@@ -681,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
+    <sheetView zoomScale="237" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -840,9 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1216,7 +1214,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix definitivo logo commferr.png, aggiorno sponsor e Excel
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B90272C-C8E9-F240-BAA4-938FB824FF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6318CF-774F-8840-B471-C8C19500F083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
@@ -840,7 +840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0"/>
+    <sheetView topLeftCell="F1" zoomScale="342" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1213,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
About: card moderna con bottoni Instagram e download regolamento; aggiornati immagini, PDF ed Excel
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6318CF-774F-8840-B471-C8C19500F083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD36BEB2-8B92-1E44-BB55-AD7315F186C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="53">
   <si>
     <t>Data</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Caffè Bistrot Mini</t>
-  </si>
-  <si>
-    <t>Commerciali Ferramenta</t>
   </si>
   <si>
     <t>Bar Caligo Spazio Kura</t>
@@ -651,7 +648,7 @@
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="13">
         <v>0.85416666666666663</v>
@@ -663,13 +660,13 @@
         <v>31</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -681,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="237" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -707,7 +704,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -735,7 +732,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -791,7 +788,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -840,7 +837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="342" workbookViewId="0">
+    <sheetView zoomScale="342" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -918,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -953,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -961,7 +958,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -988,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1023,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1058,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1093,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1101,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
@@ -1128,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1163,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1198,12 +1195,12 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1215,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="190" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1269,13 +1266,13 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -1292,16 +1289,16 @@
         <v>27</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -1321,13 +1318,13 @@
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -1347,13 +1344,13 @@
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
         <v>30</v>
@@ -1373,13 +1370,13 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>48</v>
-      </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
         <v>30</v>
@@ -1396,16 +1393,16 @@
         <v>28</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -1422,16 +1419,16 @@
         <v>27</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
         <v>52</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
         <v>30</v>
@@ -1451,13 +1448,13 @@
         <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
         <v>30</v>
@@ -1474,16 +1471,16 @@
         <v>28</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
@@ -1491,7 +1488,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2">
         <v>0.85416666666666663</v>
@@ -1503,13 +1500,13 @@
         <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s">
         <v>30</v>
@@ -1517,7 +1514,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2">
         <v>0.89583333333333337</v>
@@ -1529,13 +1526,13 @@
         <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -1552,16 +1549,16 @@
         <v>28</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>32</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" t="s">
         <v>30</v>
@@ -1581,13 +1578,13 @@
         <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -1607,13 +1604,13 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" t="s">
         <v>30</v>
@@ -1633,13 +1630,13 @@
         <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" t="s">
         <v>52</v>
-      </c>
-      <c r="G16" t="s">
-        <v>53</v>
       </c>
       <c r="H16" t="s">
         <v>30</v>
@@ -1659,13 +1656,13 @@
         <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H17" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Aggiorno file Excel torneo
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0303DC-170D-E043-A396-443A1094DAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CE3420-1EBD-1848-820A-605AC6626AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="133">
   <si>
     <t>Data</t>
   </si>
@@ -419,6 +419,9 @@
   </si>
   <si>
     <t>Marco Astolfi</t>
+  </si>
+  <si>
+    <t>Elmehdi</t>
   </si>
 </sst>
 </file>
@@ -697,7 +700,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1080,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="217" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="217" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2436,6 +2439,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B80" t="s">
+        <v>132</v>
+      </c>
+      <c r="C80" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" t="s">
+        <v>46</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2445,7 +2465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+    <sheetView zoomScale="189" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -2820,7 +2840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="190" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="190" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Aggiorno file e asset statici
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CE3420-1EBD-1848-820A-605AC6626AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FB2D04-3053-E04C-A8EB-66F10EC441A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="134">
   <si>
     <t>Data</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>Elmehdi</t>
+  </si>
+  <si>
+    <t>Maicol Batti</t>
   </si>
 </sst>
 </file>
@@ -1083,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="217" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="217" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1094,6 +1097,7 @@
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1297,7 +1301,7 @@
         <v>23</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1348,7 +1352,7 @@
         <v>45</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2195,7 +2199,7 @@
         <v>12</v>
       </c>
       <c r="D65">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2212,7 +2216,7 @@
         <v>13</v>
       </c>
       <c r="D66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -2305,16 +2309,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B72" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C72" t="s">
-        <v>13</v>
-      </c>
-      <c r="D72" t="s">
-        <v>72</v>
+        <v>11</v>
+      </c>
+      <c r="D72">
+        <v>7</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -2325,10 +2329,10 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C73" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D73" t="s">
         <v>72</v>
@@ -2338,11 +2342,11 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="39" t="s">
-        <v>35</v>
+      <c r="A74" t="s">
+        <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C74" t="s">
         <v>11</v>
@@ -2359,10 +2363,10 @@
         <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C75" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D75" t="s">
         <v>72</v>
@@ -2376,7 +2380,7 @@
         <v>35</v>
       </c>
       <c r="B76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C76" t="s">
         <v>13</v>
@@ -2393,7 +2397,7 @@
         <v>35</v>
       </c>
       <c r="B77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C77" t="s">
         <v>13</v>
@@ -2410,7 +2414,7 @@
         <v>35</v>
       </c>
       <c r="B78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C78" t="s">
         <v>13</v>
@@ -2427,10 +2431,10 @@
         <v>35</v>
       </c>
       <c r="B79" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D79" t="s">
         <v>72</v>
@@ -2441,18 +2445,35 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="39" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C80" t="s">
         <v>12</v>
       </c>
       <c r="D80" t="s">
+        <v>72</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B81" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" t="s">
         <v>46</v>
       </c>
-      <c r="E80">
+      <c r="E81">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nuovo commit di aggiornamento file
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FB2D04-3053-E04C-A8EB-66F10EC441A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE61328F-A2B6-054A-8CD0-0221EC0A9920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="217" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="217" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1352,7 +1352,7 @@
         <v>45</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Nuovo aggiornamento dati e file statici
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE61328F-A2B6-054A-8CD0-0221EC0A9920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E961B8-CC1A-F241-B619-14B64197F229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="135">
   <si>
     <t>Data</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t>Maicol Batti</t>
+  </si>
+  <si>
+    <t>0-4</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1021,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1088,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="217" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="217" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1352,7 +1355,7 @@
         <v>45</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2861,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="190" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2950,7 +2953,7 @@
         <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Aggiornamento ulteriore dati e file statici
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E961B8-CC1A-F241-B619-14B64197F229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87796D4-41E0-124D-82C5-B61A8F353396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
     <t>Maicol Batti</t>
   </si>
   <si>
-    <t>0-4</t>
+    <t>0-5</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="217" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="217" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1355,7 +1355,7 @@
         <v>45</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2864,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="D1" zoomScale="190" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Aggiornamento fine prima parita
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9315C110-E922-C743-95EA-CE78E4A6FE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB45360-466B-0B4F-AA47-60A52852AE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
@@ -2489,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView zoomScale="189" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2546,10 +2546,10 @@
         <v>24</v>
       </c>
       <c r="D2" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="15">
         <v>0</v>
@@ -2564,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>39</v>
@@ -2616,7 +2616,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="18">
         <v>0</v>
@@ -2625,7 +2625,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="34">
         <v>0</v>
@@ -2864,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="D1" zoomScale="190" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Versione con risultati colorati
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/WEB DEV/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FA5311-DD37-7F4E-BDFD-795FF1A81D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDACF12-A190-DE4D-BDA6-5B7CB5FBD351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
@@ -712,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -804,6 +804,10 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,7 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
@@ -3322,8 +3326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3334,6 +3338,7 @@
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="32.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -3358,7 +3363,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="53" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3384,7 +3389,7 @@
       <c r="G2" t="s">
         <v>154</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="54" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3410,7 +3415,7 @@
       <c r="G3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="54" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3436,7 +3441,7 @@
       <c r="G4" t="s">
         <v>40</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3462,7 +3467,7 @@
       <c r="G5" t="s">
         <v>154</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3488,7 +3493,7 @@
       <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3514,7 +3519,7 @@
       <c r="G7" t="s">
         <v>38</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3540,7 +3545,7 @@
       <c r="G8" t="s">
         <v>40</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3566,7 +3571,7 @@
       <c r="G9" t="s">
         <v>41</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3592,7 +3597,7 @@
       <c r="G10" t="s">
         <v>42</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3618,7 +3623,7 @@
       <c r="G11" t="s">
         <v>39</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3644,7 +3649,7 @@
       <c r="G12" t="s">
         <v>41</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3670,7 +3675,7 @@
       <c r="G13" t="s">
         <v>37</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3696,7 +3701,7 @@
       <c r="G14" t="s">
         <v>36</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3722,7 +3727,7 @@
       <c r="G15" t="s">
         <v>36</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3748,7 +3753,7 @@
       <c r="G16" t="s">
         <v>44</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3774,7 +3779,7 @@
       <c r="G17" t="s">
         <v>154</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="54" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correzione gol su ricerca
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/WEB DEV/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDACF12-A190-DE4D-BDA6-5B7CB5FBD351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B029F0F5-ADB2-024E-8012-E1472111CE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3326,8 +3326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="C20" sqref="C18:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
chore: aggiorno anche DATITORNEO.xlsx e tutti i file per deploy online
</commit_message>
<xml_diff>
--- a/DATITORNEO.xlsx
+++ b/DATITORNEO.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto.libanora/Desktop/WEB DEV/torneoapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43FB0E1-783D-6A49-AC8E-BAA3213593D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D05A66-5329-414E-9753-09E2ABF43B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prossime Partite" sheetId="1" r:id="rId1"/>
     <sheet name="Rose" sheetId="2" r:id="rId2"/>
     <sheet name="Classifiche" sheetId="3" r:id="rId3"/>
     <sheet name="Calendario Partite" sheetId="4" r:id="rId4"/>
+    <sheet name="Finale" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="173">
   <si>
     <t>Data</t>
   </si>
@@ -514,9 +515,6 @@
     <t>Finalista 2</t>
   </si>
   <si>
-    <t>Giulio Pico</t>
-  </si>
-  <si>
     <t>7-4</t>
   </si>
   <si>
@@ -539,6 +537,12 @@
   </si>
   <si>
     <t>N-N</t>
+  </si>
+  <si>
+    <t>Vincitore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -548,7 +552,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -576,6 +580,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -643,7 +655,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -676,6 +688,17 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -749,10 +772,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1094,30 +1119,35 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="33" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>45855</v>
+        <v>45856</v>
       </c>
       <c r="B2" s="2">
         <v>0.875</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
+        <v>161</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>159</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="16"/>
+        <v>162</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1126,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="234" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A40" zoomScale="234" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2012,33 +2042,33 @@
         <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D52">
         <v>11</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" t="s">
-        <v>65</v>
+        <v>44</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2046,13 +2076,13 @@
         <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -2063,16 +2093,16 @@
         <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D55">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2080,16 +2110,16 @@
         <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2097,16 +2127,16 @@
         <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C57" t="s">
         <v>13</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2114,16 +2144,16 @@
         <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D58">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2131,13 +2161,13 @@
         <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D59">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -2148,16 +2178,16 @@
         <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D60">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2165,16 +2195,16 @@
         <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D61">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E61">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2182,16 +2212,16 @@
         <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D62">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2199,13 +2229,13 @@
         <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="C63" t="s">
         <v>12</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -2213,16 +2243,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B64" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D64">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -2233,13 +2263,13 @@
         <v>41</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2250,16 +2280,16 @@
         <v>41</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C66" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2267,16 +2297,16 @@
         <v>41</v>
       </c>
       <c r="B67" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D67">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -2284,13 +2314,13 @@
         <v>41</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C68" t="s">
         <v>12</v>
       </c>
       <c r="D68">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -2301,13 +2331,13 @@
         <v>41</v>
       </c>
       <c r="B69" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D69">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -2318,13 +2348,13 @@
         <v>41</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D70">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -2335,13 +2365,13 @@
         <v>41</v>
       </c>
       <c r="B71" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -2352,13 +2382,13 @@
         <v>41</v>
       </c>
       <c r="B72" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C72" t="s">
         <v>11</v>
       </c>
       <c r="D72">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -2369,16 +2399,16 @@
         <v>41</v>
       </c>
       <c r="B73" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73">
         <v>11</v>
       </c>
-      <c r="D73">
-        <v>10</v>
-      </c>
       <c r="E73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2386,16 +2416,16 @@
         <v>41</v>
       </c>
       <c r="B74" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C74" t="s">
+        <v>156</v>
+      </c>
+      <c r="D74">
         <v>12</v>
       </c>
-      <c r="D74">
-        <v>11</v>
-      </c>
       <c r="E74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -2403,33 +2433,33 @@
         <v>41</v>
       </c>
       <c r="B75" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C75" t="s">
-        <v>156</v>
+        <v>11</v>
       </c>
       <c r="D75">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>41</v>
+      <c r="A76" s="13" t="s">
+        <v>149</v>
       </c>
       <c r="B76" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C76" t="s">
         <v>11</v>
       </c>
       <c r="D76">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2437,16 +2467,16 @@
         <v>149</v>
       </c>
       <c r="B77" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="C77" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D77">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E77">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2454,16 +2484,16 @@
         <v>149</v>
       </c>
       <c r="B78" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C78" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D78">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="E78">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2471,13 +2501,13 @@
         <v>149</v>
       </c>
       <c r="B79" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D79">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -2488,13 +2518,13 @@
         <v>149</v>
       </c>
       <c r="B80" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C80" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D80">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -2505,13 +2535,13 @@
         <v>149</v>
       </c>
       <c r="B81" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -2522,13 +2552,13 @@
         <v>149</v>
       </c>
       <c r="B82" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C82" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D82">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2539,13 +2569,13 @@
         <v>149</v>
       </c>
       <c r="B83" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="C83" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D83">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -2556,13 +2586,13 @@
         <v>149</v>
       </c>
       <c r="B84" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D84">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -2573,13 +2603,13 @@
         <v>149</v>
       </c>
       <c r="B85" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C85" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D85">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -2590,13 +2620,13 @@
         <v>149</v>
       </c>
       <c r="B86" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="C86" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -2607,16 +2637,16 @@
         <v>149</v>
       </c>
       <c r="B87" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="C87" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D87">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2624,30 +2654,30 @@
         <v>149</v>
       </c>
       <c r="B88" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C88" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D88">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
       <c r="B89" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C89" t="s">
         <v>44</v>
       </c>
       <c r="D89">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="E89">
         <v>0</v>
@@ -2658,13 +2688,13 @@
         <v>33</v>
       </c>
       <c r="B90" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C90" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -2675,16 +2705,16 @@
         <v>33</v>
       </c>
       <c r="B91" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C91" t="s">
         <v>13</v>
       </c>
       <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91">
         <v>2</v>
-      </c>
-      <c r="E91">
-        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2692,16 +2722,16 @@
         <v>33</v>
       </c>
       <c r="B92" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="C92" t="s">
         <v>13</v>
       </c>
       <c r="D92">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2709,13 +2739,13 @@
         <v>33</v>
       </c>
       <c r="B93" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D93">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -2726,16 +2756,16 @@
         <v>33</v>
       </c>
       <c r="B94" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="C94" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D94">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2743,16 +2773,16 @@
         <v>33</v>
       </c>
       <c r="B95" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C95" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D95">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2760,16 +2790,16 @@
         <v>33</v>
       </c>
       <c r="B96" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D96">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E96">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -2777,16 +2807,16 @@
         <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C97" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D97">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E97">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -2794,16 +2824,16 @@
         <v>33</v>
       </c>
       <c r="B98" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C98" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98">
         <v>11</v>
       </c>
-      <c r="D98">
-        <v>17</v>
-      </c>
       <c r="E98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -2811,16 +2841,16 @@
         <v>33</v>
       </c>
       <c r="B99" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C99" t="s">
         <v>12</v>
       </c>
       <c r="D99">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -2828,16 +2858,16 @@
         <v>33</v>
       </c>
       <c r="B100" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="C100" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D100">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E100">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -2845,37 +2875,20 @@
         <v>33</v>
       </c>
       <c r="B101" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C101" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D101">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B102" t="s">
-        <v>153</v>
-      </c>
-      <c r="C102" t="s">
-        <v>12</v>
-      </c>
-      <c r="D102">
-        <v>2</v>
-      </c>
-      <c r="E102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="13"/>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3278,8 +3291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3524,7 +3537,7 @@
         <v>36</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3550,7 +3563,7 @@
         <v>35</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3576,7 +3589,7 @@
         <v>136</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -3602,7 +3615,7 @@
         <v>42</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -3613,7 +3626,7 @@
         <v>0.9375</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>32</v>
@@ -3628,7 +3641,7 @@
         <v>136</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -3715,13 +3728,6 @@
       <c r="J17" s="7"/>
       <c r="O17" s="16"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C21" s="33"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-    </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="6"/>
     </row>
@@ -3743,4 +3749,37 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D2EB7B-07A7-8143-8E19-A55CDA8FD46C}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView zoomScale="183" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>